<commit_message>
Check login va bao cao, user he thong
</commit_message>
<xml_diff>
--- a/Api.ManagerGift/TempExport/Bao Cao Ton Kho.xlsx
+++ b/Api.ManagerGift/TempExport/Bao Cao Ton Kho.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA97C17-BE7F-4D80-9665-B75C60E74EC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Xuat kho qua tang" sheetId="2" r:id="rId1"/>
@@ -15,51 +14,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>BÁO CÁO QUÀ TẶNG XUẤT KHO</t>
-  </si>
-  <si>
-    <t>Từ ngày.........đến ngày............</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Tên quà tặng</t>
-  </si>
-  <si>
-    <t>Mã quà tặng</t>
-  </si>
-  <si>
     <t>Số lượng</t>
   </si>
   <si>
-    <t>Đơn vị tính</t>
-  </si>
-  <si>
-    <t>Giá trị</t>
-  </si>
-  <si>
-    <t>Thành tiền</t>
-  </si>
-  <si>
-    <t>Ngày tạo</t>
-  </si>
-  <si>
-    <t>Tên kho nhập</t>
-  </si>
-  <si>
-    <t>Tên kho xuất</t>
-  </si>
-  <si>
-    <t>Ghi chú</t>
+    <t>BÁO CÁO QUÀ TẶNG TỒN KHO</t>
+  </si>
+  <si>
+    <t>Đơn vị</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ngày …</t>
+  </si>
+  <si>
+    <t>Chương trình khuyến mãi</t>
+  </si>
+  <si>
+    <t>Quà tặng</t>
+  </si>
+  <si>
+    <t>Ngày</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -137,24 +121,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -167,12 +138,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -180,6 +145,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -274,23 +251,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -326,23 +286,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -518,125 +461,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AF528D-71AB-4BC7-9A2D-A451951AFBDC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="10" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="10" width="14.85546875" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>